<commit_message>
eddy ni 1993-1994 (update 3)
</commit_message>
<xml_diff>
--- a/_data/ni/ni9394/individueel_eindstand_dworp_123_9394.xlsx
+++ b/_data/ni/ni9394/individueel_eindstand_dworp_123_9394.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14505" yWindow="-15" windowWidth="14310" windowHeight="12840" activeTab="10"/>
+    <workbookView xWindow="14505" yWindow="-15" windowWidth="14310" windowHeight="12840" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -2672,7 +2672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -14633,8 +14633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14760,13 +14760,13 @@
         <v>1900</v>
       </c>
       <c r="E6" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="14" t="s">
@@ -14871,13 +14871,13 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="13">
         <v>1.5</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="13">
-        <v>2.5</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="16" t="str">

</xml_diff>

<commit_message>
eddy ni 1993-1994 (update 5)
</commit_message>
<xml_diff>
--- a/_data/ni/ni9394/individueel_eindstand_dworp_123_9394.xlsx
+++ b/_data/ni/ni9394/individueel_eindstand_dworp_123_9394.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14505" yWindow="-15" windowWidth="14310" windowHeight="12840"/>
+    <workbookView xWindow="14505" yWindow="-15" windowWidth="14310" windowHeight="12840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -301,9 +301,6 @@
     <t>Barthelemy René</t>
   </si>
   <si>
-    <t>Matthys Luc</t>
-  </si>
-  <si>
     <t>418 Geraardsbergen 2</t>
   </si>
   <si>
@@ -728,6 +725,9 @@
   </si>
   <si>
     <t>Broekhuizen Peter</t>
+  </si>
+  <si>
+    <t>Matthijs Kris</t>
   </si>
 </sst>
 </file>
@@ -1802,7 +1802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1892,7 +1892,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="B13" s="71" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C13" s="71"/>
       <c r="D13" s="71"/>
@@ -1908,7 +1908,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="B14" s="71" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C14" s="71"/>
       <c r="D14" s="71"/>
@@ -1918,7 +1918,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="B15" s="71" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C15" s="71"/>
       <c r="D15" s="71"/>
@@ -1988,7 +1988,7 @@
         <v>13</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -2048,7 +2048,7 @@
         <v>25992</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J5" s="18">
         <v>1735</v>
@@ -2080,7 +2080,7 @@
         <v>68195</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J6" s="18">
         <v>1774</v>
@@ -2227,7 +2227,7 @@
         <v>13</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -2287,7 +2287,7 @@
         <v>76791</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J15" s="18">
         <v>1664</v>
@@ -2319,7 +2319,7 @@
         <v>60</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J16" s="18">
         <v>1633</v>
@@ -2351,7 +2351,7 @@
         <v>13765</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J17" s="18">
         <v>1585</v>
@@ -2383,7 +2383,7 @@
         <v>41777</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J18" s="18" t="s">
         <v>58</v>
@@ -2434,7 +2434,7 @@
         <v>13</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -2558,7 +2558,7 @@
         <v>40151</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J25" s="18">
         <v>1654</v>
@@ -2800,7 +2800,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2852,7 +2852,7 @@
         <v>68942</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D5" s="18">
         <v>2013</v>
@@ -2884,7 +2884,7 @@
         <v>81604</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D6" s="18">
         <v>2002</v>
@@ -2916,7 +2916,7 @@
         <v>91201</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D7" s="18">
         <v>1914</v>
@@ -2948,7 +2948,7 @@
         <v>94099</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D8" s="18">
         <v>1917</v>
@@ -3039,7 +3039,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -3091,7 +3091,7 @@
         <v>54500</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D15" s="18">
         <v>1892</v>
@@ -3123,7 +3123,7 @@
         <v>10961</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D16" s="18">
         <v>1885</v>
@@ -3187,7 +3187,7 @@
         <v>3174</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D18" s="18">
         <v>1752</v>
@@ -3246,7 +3246,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -3298,7 +3298,7 @@
         <v>69825</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D23" s="18">
         <v>1771</v>
@@ -3330,7 +3330,7 @@
         <v>69744</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D24" s="18">
         <v>1735</v>
@@ -3362,7 +3362,7 @@
         <v>86291</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D25" s="18">
         <v>1738</v>
@@ -3394,7 +3394,7 @@
         <v>67415</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>58</v>
@@ -3630,7 +3630,7 @@
         <v>13</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -3722,7 +3722,7 @@
         <v>81523</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J6" s="18">
         <v>1884</v>
@@ -3754,7 +3754,7 @@
         <v>71081</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J7" s="18">
         <v>1847</v>
@@ -3786,7 +3786,7 @@
         <v>71412</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J8" s="18">
         <v>1770</v>
@@ -3869,7 +3869,7 @@
         <v>13</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -3929,7 +3929,7 @@
         <v>36056</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J15" s="18">
         <v>1941</v>
@@ -3961,7 +3961,7 @@
         <v>1589</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J16" s="18">
         <v>1866</v>
@@ -3993,7 +3993,7 @@
         <v>50369</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J17" s="18">
         <v>1828</v>
@@ -4025,7 +4025,7 @@
         <v>47490</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J18" s="18">
         <v>1858</v>
@@ -4076,7 +4076,7 @@
         <v>13</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -4168,7 +4168,7 @@
         <v>64424</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J24" s="18">
         <v>1438</v>
@@ -4200,7 +4200,7 @@
         <v>67164</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J25" s="18">
         <v>1363</v>
@@ -4232,7 +4232,7 @@
         <v>64874</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J26" s="18">
         <v>1293</v>
@@ -4512,7 +4512,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C4" s="40" t="s">
         <v>79</v>
@@ -4663,7 +4663,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C5" s="41">
         <v>2.5</v>
@@ -4965,7 +4965,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C7" s="41">
         <v>1</v>
@@ -5116,7 +5116,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C8" s="41">
         <v>2</v>
@@ -5267,7 +5267,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C9" s="41">
         <v>0</v>
@@ -5418,7 +5418,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C10" s="41">
         <v>1.5</v>
@@ -5569,7 +5569,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C11" s="41">
         <v>0.5</v>
@@ -5720,7 +5720,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C12" s="41">
         <v>1</v>
@@ -6022,7 +6022,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C14" s="41">
         <v>0.5</v>
@@ -6173,7 +6173,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15" s="51">
         <v>1</v>
@@ -6406,7 +6406,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C18" s="40" t="s">
         <v>79</v>
@@ -6557,7 +6557,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C19" s="41">
         <v>3</v>
@@ -6708,7 +6708,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C20" s="41">
         <v>2</v>
@@ -7010,7 +7010,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C22" s="41">
         <v>1</v>
@@ -7161,7 +7161,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" s="41">
         <v>1.5</v>
@@ -7313,7 +7313,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C24" s="41">
         <v>1.5</v>
@@ -7464,7 +7464,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C25" s="41">
         <v>2</v>
@@ -7615,7 +7615,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C26" s="41">
         <v>0.5</v>
@@ -7766,7 +7766,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C27" s="41">
         <v>2</v>
@@ -7917,7 +7917,7 @@
         <v>11</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C28" s="41">
         <v>1.5</v>
@@ -8068,7 +8068,7 @@
         <v>12</v>
       </c>
       <c r="B29" s="50" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C29" s="51">
         <v>0</v>
@@ -8301,7 +8301,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C32" s="40" t="s">
         <v>79</v>
@@ -8452,7 +8452,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C33" s="41">
         <v>1.5</v>
@@ -8755,7 +8755,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C35" s="41">
         <v>0</v>
@@ -8906,7 +8906,7 @@
         <v>5</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C36" s="41">
         <v>1.5</v>
@@ -9057,7 +9057,7 @@
         <v>6</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C37" s="41">
         <v>0.5</v>
@@ -9208,7 +9208,7 @@
         <v>7</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C38" s="41">
         <v>1</v>
@@ -9359,7 +9359,7 @@
         <v>8</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C39" s="41">
         <v>1.5</v>
@@ -9510,7 +9510,7 @@
         <v>9</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C40" s="41">
         <v>1</v>
@@ -9661,7 +9661,7 @@
         <v>10</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C41" s="41">
         <v>1.5</v>
@@ -9812,7 +9812,7 @@
         <v>11</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C42" s="41">
         <v>1.5</v>
@@ -9963,7 +9963,7 @@
         <v>12</v>
       </c>
       <c r="B43" s="50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C43" s="51">
         <v>0</v>
@@ -11726,8 +11726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11851,7 +11851,7 @@
         <v>31381</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D6" s="18">
         <v>1787</v>
@@ -12006,7 +12006,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -12055,13 +12055,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="19">
-        <v>19208</v>
+        <v>46345</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>91</v>
+        <v>233</v>
       </c>
       <c r="D15" s="18">
-        <v>1975</v>
+        <v>1934</v>
       </c>
       <c r="E15" s="10">
         <v>0.5</v>
@@ -12090,7 +12090,7 @@
         <v>32794</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D16" s="18">
         <v>1957</v>
@@ -12122,7 +12122,7 @@
         <v>30732</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D17" s="18">
         <v>1836</v>
@@ -12154,7 +12154,7 @@
         <v>61476</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D18" s="18">
         <v>1757</v>
@@ -12183,7 +12183,7 @@
       <c r="B19" s="3"/>
       <c r="C19" s="16">
         <f>IFERROR(AVERAGE(D15:D18),"")</f>
-        <v>1881.25</v>
+        <v>1871</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="13">
@@ -12213,7 +12213,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -12599,7 +12599,7 @@
         <v>13</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -12691,7 +12691,7 @@
         <v>85928</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J6" s="18">
         <v>1845</v>
@@ -12723,7 +12723,7 @@
         <v>40274</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J7" s="18">
         <v>1823</v>
@@ -12755,7 +12755,7 @@
         <v>1279</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J8" s="18">
         <v>1798</v>
@@ -12838,7 +12838,7 @@
         <v>13</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -12898,7 +12898,7 @@
         <v>17515</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J15" s="18">
         <v>1775</v>
@@ -12924,13 +12924,13 @@
         <v>11</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H16" s="19">
         <v>12556</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J16" s="18">
         <v>1744</v>
@@ -12962,7 +12962,7 @@
         <v>96431</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J17" s="18">
         <v>1731</v>
@@ -13045,7 +13045,7 @@
         <v>13</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -13105,7 +13105,7 @@
         <v>60097</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J23" s="18">
         <v>1693</v>
@@ -13137,7 +13137,7 @@
         <v>66346</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J24" s="18">
         <v>1568</v>
@@ -13201,7 +13201,7 @@
         <v>58025</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J26" s="18">
         <v>1430</v>
@@ -13409,7 +13409,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -13461,7 +13461,7 @@
         <v>71676</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5" s="18">
         <v>2021</v>
@@ -13493,7 +13493,7 @@
         <v>82210</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D6" s="18">
         <v>1921</v>
@@ -13525,7 +13525,7 @@
         <v>63193</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D7" s="18">
         <v>1854</v>
@@ -13557,7 +13557,7 @@
         <v>97781</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D8" s="18">
         <v>1831</v>
@@ -13648,7 +13648,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -13700,7 +13700,7 @@
         <v>53449</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D15" s="18">
         <v>1979</v>
@@ -13732,7 +13732,7 @@
         <v>22080</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D16" s="18">
         <v>1964</v>
@@ -13796,7 +13796,7 @@
         <v>49689</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D18" s="18">
         <v>1797</v>
@@ -13855,7 +13855,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -13907,7 +13907,7 @@
         <v>64157</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D23" s="18">
         <v>1668</v>
@@ -13939,7 +13939,7 @@
         <v>73695</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D24" s="18">
         <v>1638</v>
@@ -13971,7 +13971,7 @@
         <v>73741</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D25" s="18">
         <v>1629</v>
@@ -14003,7 +14003,7 @@
         <v>78549</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D26" s="18">
         <v>1577</v>
@@ -14229,7 +14229,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -14281,7 +14281,7 @@
         <v>80918</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5" s="18">
         <v>1869</v>
@@ -14313,7 +14313,7 @@
         <v>93688</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D6" s="18">
         <v>1824</v>
@@ -14345,7 +14345,7 @@
         <v>79669</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D7" s="18">
         <v>1751</v>
@@ -14377,7 +14377,7 @@
         <v>67539</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D8" s="18">
         <v>1658</v>
@@ -14468,7 +14468,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -14520,7 +14520,7 @@
         <v>26492</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D15" s="18">
         <v>1892</v>
@@ -14552,7 +14552,7 @@
         <v>31895</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D16" s="18">
         <v>1775</v>
@@ -14584,7 +14584,7 @@
         <v>22519</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D17" s="18">
         <v>1680</v>
@@ -14616,7 +14616,7 @@
         <v>47589</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>58</v>
@@ -14675,7 +14675,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -14727,7 +14727,7 @@
         <v>18767</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D23" s="18">
         <v>2122</v>
@@ -14759,7 +14759,7 @@
         <v>55816</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D24" s="18">
         <v>1553</v>
@@ -14791,7 +14791,7 @@
         <v>88994</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D25" s="18">
         <v>1419</v>
@@ -14823,7 +14823,7 @@
         <v>62391</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D26" s="18">
         <v>1278</v>
@@ -15059,7 +15059,7 @@
         <v>13</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -15119,7 +15119,7 @@
         <v>63134</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J5" s="18">
         <v>1958</v>
@@ -15151,7 +15151,7 @@
         <v>44261</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J6" s="18">
         <v>1883</v>
@@ -15183,7 +15183,7 @@
         <v>61280</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J7" s="18">
         <v>1875</v>
@@ -15215,7 +15215,7 @@
         <v>70114</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J8" s="18" t="s">
         <v>58</v>
@@ -15298,7 +15298,7 @@
         <v>13</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -15358,7 +15358,7 @@
         <v>17043</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J15" s="18">
         <v>1932</v>
@@ -15390,7 +15390,7 @@
         <v>45314</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J16" s="18">
         <v>1792</v>
@@ -15422,7 +15422,7 @@
         <v>13510</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J17" s="18">
         <v>1745</v>
@@ -15454,7 +15454,7 @@
         <v>46604</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J18" s="18" t="s">
         <v>58</v>
@@ -15505,7 +15505,7 @@
         <v>13</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -15565,7 +15565,7 @@
         <v>94901</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J23" s="18">
         <v>1523</v>
@@ -15597,7 +15597,7 @@
         <v>63274</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J24" s="18">
         <v>1429</v>
@@ -15629,7 +15629,7 @@
         <v>89729</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J25" s="18">
         <v>1418</v>
@@ -15661,7 +15661,7 @@
         <v>68497</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J26" s="18" t="s">
         <v>58</v>
@@ -15869,7 +15869,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -15921,7 +15921,7 @@
         <v>74888</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D5" s="18">
         <v>1890</v>
@@ -15953,7 +15953,7 @@
         <v>55671</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D6" s="18">
         <v>1803</v>
@@ -15985,7 +15985,7 @@
         <v>84573</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D7" s="18">
         <v>1517</v>
@@ -16017,7 +16017,7 @@
         <v>86002</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D8" s="18">
         <v>1614</v>
@@ -16108,7 +16108,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -16160,7 +16160,7 @@
         <v>21938</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D15" s="18">
         <v>2117</v>
@@ -16192,7 +16192,7 @@
         <v>89265</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D16" s="18">
         <v>2067</v>
@@ -16224,7 +16224,7 @@
         <v>21717</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D17" s="18">
         <v>1988</v>
@@ -16256,7 +16256,7 @@
         <v>41955</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D18" s="18">
         <v>1968</v>
@@ -16315,7 +16315,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -16367,7 +16367,7 @@
         <v>86070</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D23" s="18">
         <v>1468</v>
@@ -16399,7 +16399,7 @@
         <v>50580</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D24" s="18">
         <v>1090</v>
@@ -16431,7 +16431,7 @@
         <v>61034</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>58</v>
@@ -16463,7 +16463,7 @@
         <v>58629</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>58</v>
@@ -16699,7 +16699,7 @@
         <v>13</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -16759,7 +16759,7 @@
         <v>49034</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J5" s="18">
         <v>1814</v>
@@ -16791,7 +16791,7 @@
         <v>74225</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J6" s="18">
         <v>1808</v>
@@ -16823,7 +16823,7 @@
         <v>93181</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J7" s="18">
         <v>1742</v>
@@ -16855,7 +16855,7 @@
         <v>28673</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J8" s="18">
         <v>1764</v>
@@ -16938,7 +16938,7 @@
         <v>13</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -17145,7 +17145,7 @@
         <v>13</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -17173,7 +17173,7 @@
         <v>14</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J22" s="9" t="s">
         <v>7</v>
@@ -17205,7 +17205,7 @@
         <v>73865</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J23" s="18">
         <v>1758</v>
@@ -17269,7 +17269,7 @@
         <v>4251</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J25" s="18">
         <v>1293</v>
@@ -17301,7 +17301,7 @@
         <v>59994</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J26" s="18">
         <v>823</v>
@@ -17511,7 +17511,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -17563,7 +17563,7 @@
         <v>72460</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D5" s="18">
         <v>2090</v>
@@ -17595,7 +17595,7 @@
         <v>89516</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D6" s="18">
         <v>1987</v>
@@ -17627,7 +17627,7 @@
         <v>95753</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D7" s="18">
         <v>2031</v>
@@ -17659,7 +17659,7 @@
         <v>68721</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D8" s="18">
         <v>1935</v>
@@ -17750,7 +17750,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -17802,7 +17802,7 @@
         <v>604</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D15" s="18">
         <v>2025</v>
@@ -17898,7 +17898,7 @@
         <v>2941</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D18" s="18">
         <v>1631</v>
@@ -17957,7 +17957,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -18009,7 +18009,7 @@
         <v>11355</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D23" s="18">
         <v>1699</v>
@@ -18041,7 +18041,7 @@
         <v>80292</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D24" s="18">
         <v>1568</v>
@@ -18073,7 +18073,7 @@
         <v>25798</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D25" s="18">
         <v>1400</v>

</xml_diff>